<commit_message>
add nokia id info
</commit_message>
<xml_diff>
--- a/01_FBs_Plan.xlsx
+++ b/01_FBs_Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\changpzh\01_nokia_work\03_megaZone\16_SM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\changpzh\01_nokia_work\90_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -858,7 +858,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -1407,21 +1407,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1627,6 +1612,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1636,7 +1649,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1883,61 +1896,58 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -2027,12 +2037,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2045,49 +2055,61 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="59" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="60" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2095,7 +2117,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FFBA40A9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2148,12 +2180,12 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFBA40A9"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF7030A0"/>
       </font>
     </dxf>
     <dxf>
@@ -2595,21 +2627,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E83" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E83" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A1:E83"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Module" dataDxfId="36"/>
-    <tableColumn id="2" name="Task" dataDxfId="35"/>
+    <tableColumn id="1" name="Module" dataDxfId="38"/>
+    <tableColumn id="2" name="Task" dataDxfId="37"/>
     <tableColumn id="6" name="Priority"/>
-    <tableColumn id="3" name="Owner" dataDxfId="34"/>
-    <tableColumn id="5" name="EE" dataDxfId="33"/>
+    <tableColumn id="3" name="Owner" dataDxfId="36"/>
+    <tableColumn id="5" name="EE" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:E100" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:E100" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="A1:E100"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Module"/>
@@ -2623,7 +2655,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:E100" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:E100" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="A1:E100"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Module"/>
@@ -2637,7 +2669,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table158" displayName="Table158" ref="A1:E100" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table158" displayName="Table158" ref="A1:E100" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="A1:E100"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Module"/>
@@ -2953,536 +2985,544 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="7.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="7.77734375" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="144" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="141" t="s">
+      <c r="B1" s="144" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="141" t="s">
+      <c r="C1" s="144" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="141" t="s">
+      <c r="D1" s="144" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="139" t="s">
+      <c r="E1" s="150" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="143"/>
-      <c r="G1" s="139" t="s">
+      <c r="F1" s="142"/>
+      <c r="G1" s="141" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="143"/>
-      <c r="I1" s="139" t="s">
+      <c r="H1" s="142"/>
+      <c r="I1" s="141" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="143"/>
-      <c r="K1" s="139" t="s">
+      <c r="J1" s="142"/>
+      <c r="K1" s="141" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="143"/>
-      <c r="M1" s="139" t="s">
+      <c r="L1" s="142"/>
+      <c r="M1" s="141" t="s">
         <v>148</v>
       </c>
-      <c r="N1" s="143"/>
-      <c r="O1" s="139" t="s">
+      <c r="N1" s="142"/>
+      <c r="O1" s="141" t="s">
         <v>149</v>
       </c>
-      <c r="P1" s="143"/>
+      <c r="P1" s="142"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="140"/>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="91" t="s">
+      <c r="A2" s="145"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="91" t="s">
+      <c r="G2" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="H2" s="90" t="s">
+      <c r="H2" s="89" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="91" t="s">
+      <c r="I2" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="90" t="s">
+      <c r="J2" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="K2" s="91" t="s">
+      <c r="K2" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="L2" s="90" t="s">
+      <c r="L2" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="91" t="s">
+      <c r="M2" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="N2" s="90" t="s">
+      <c r="N2" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="O2" s="91" t="s">
+      <c r="O2" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="P2" s="90" t="s">
+      <c r="P2" s="89" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="146" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="83" t="s">
         <v>95</v>
       </c>
       <c r="C3" s="82">
         <v>69005657</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="130">
+      <c r="E3" s="129">
         <v>0</v>
       </c>
-      <c r="F3" s="131">
+      <c r="F3" s="130">
         <f ca="1">SUM(SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!D1:D100"), $B3,INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!E1:E100")), SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!D1:D100"), "ALL", INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!E1:E100")))</f>
         <v>78</v>
       </c>
-      <c r="G3" s="130">
+      <c r="G3" s="129">
         <v>5</v>
       </c>
-      <c r="H3" s="131">
+      <c r="H3" s="130">
         <f ca="1">SUM(SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!D1:D100"), $B3,INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!E1:E100")), SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!D1:D100"), "ALL", INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!E1:E100")))</f>
         <v>0</v>
       </c>
-      <c r="I3" s="130">
+      <c r="I3" s="129">
         <v>0</v>
       </c>
-      <c r="J3" s="131">
+      <c r="J3" s="130">
         <f ca="1">SUM(SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(J$2, SEARCH(" ", J$2)-1), "_Plans")&amp;"!D1:D100"), $B3,INDIRECT(_xlfn.CONCAT(LEFT(J$2, SEARCH(" ", J$2)-1), "_Plans")&amp;"!E1:E100")), SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(J$2, SEARCH(" ", J$2)-1), "_Plans")&amp;"!D1:D100"), "ALL", INDIRECT(_xlfn.CONCAT(LEFT(J$2, SEARCH(" ", J$2)-1), "_Plans")&amp;"!E1:E100")))</f>
         <v>0</v>
       </c>
-      <c r="K3" s="130">
+      <c r="K3" s="129">
         <v>0</v>
       </c>
-      <c r="L3" s="131">
+      <c r="L3" s="130">
         <f ca="1">SUM(SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(L$2, SEARCH(" ", L$2)-1), "_Plans")&amp;"!D1:D100"), $B3,INDIRECT(_xlfn.CONCAT(LEFT(L$2, SEARCH(" ", L$2)-1), "_Plans")&amp;"!E1:E100")), SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(L$2, SEARCH(" ", L$2)-1), "_Plans")&amp;"!D1:D100"), "ALL", INDIRECT(_xlfn.CONCAT(LEFT(L$2, SEARCH(" ", L$2)-1), "_Plans")&amp;"!E1:E100")))</f>
         <v>0</v>
       </c>
-      <c r="M3" s="86"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="88"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="4" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="146" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="85" t="s">
+      <c r="C4" s="82">
+        <v>61431860</v>
+      </c>
+      <c r="D4" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="130">
+      <c r="E4" s="129">
         <v>0</v>
       </c>
-      <c r="F4" s="131">
+      <c r="F4" s="130">
         <f t="shared" ref="F4:L9" ca="1" si="0">SUM(SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!D1:D100"), $B4,INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!E1:E100")), SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!D1:D100"), "ALL", INDIRECT(_xlfn.CONCAT(LEFT(F$2, SEARCH(" ", F$2)-1), "_Plans")&amp;"!E1:E100")))</f>
         <v>90</v>
       </c>
-      <c r="G4" s="130">
+      <c r="G4" s="129">
         <v>2</v>
       </c>
-      <c r="H4" s="131">
+      <c r="H4" s="130">
         <f ca="1">SUM(SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!D1:D100"), $B4,INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!E1:E100")), SUMIF(INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!D1:D100"), "ALL", INDIRECT(_xlfn.CONCAT(LEFT(H$2, SEARCH(" ", H$2)-1), "_Plans")&amp;"!E1:E100")))</f>
         <v>0</v>
       </c>
-      <c r="I4" s="130">
+      <c r="I4" s="129">
         <v>0</v>
       </c>
-      <c r="J4" s="131">
+      <c r="J4" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="K4" s="130">
+      <c r="K4" s="129">
         <v>0</v>
       </c>
-      <c r="L4" s="131">
+      <c r="L4" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="M4" s="89"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="87"/>
     </row>
     <row r="5" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="146" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="83" t="s">
         <v>97</v>
       </c>
       <c r="C5" s="82">
         <v>62157104</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="130">
+      <c r="E5" s="129">
         <v>0</v>
       </c>
-      <c r="F5" s="131">
+      <c r="F5" s="130">
         <v>0</v>
       </c>
-      <c r="G5" s="130">
+      <c r="G5" s="129">
         <v>0</v>
       </c>
-      <c r="H5" s="131">
+      <c r="H5" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="130">
+      <c r="I5" s="129">
         <v>0</v>
       </c>
-      <c r="J5" s="131">
+      <c r="J5" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="130">
+      <c r="K5" s="129">
         <v>0</v>
       </c>
-      <c r="L5" s="131">
+      <c r="L5" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="87"/>
     </row>
     <row r="6" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="146" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="85" t="s">
+      <c r="C6" s="82">
+        <v>62148502</v>
+      </c>
+      <c r="D6" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="130">
+      <c r="E6" s="129">
         <v>0</v>
       </c>
-      <c r="F6" s="131">
+      <c r="F6" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>130</v>
       </c>
-      <c r="G6" s="130">
+      <c r="G6" s="129">
         <v>0</v>
       </c>
-      <c r="H6" s="131">
+      <c r="H6" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="130">
+      <c r="I6" s="129">
         <v>0</v>
       </c>
-      <c r="J6" s="131">
+      <c r="J6" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="130">
+      <c r="K6" s="129">
         <v>0</v>
       </c>
-      <c r="L6" s="131">
+      <c r="L6" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="M6" s="89"/>
-      <c r="N6" s="87"/>
-      <c r="O6" s="89"/>
-      <c r="P6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="87"/>
     </row>
     <row r="7" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="146" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="85" t="s">
+      <c r="C7" s="82">
+        <v>62148507</v>
+      </c>
+      <c r="D7" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="130">
+      <c r="E7" s="129">
         <v>0</v>
       </c>
-      <c r="F7" s="131">
+      <c r="F7" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>146</v>
       </c>
-      <c r="G7" s="130">
+      <c r="G7" s="129">
         <v>0</v>
       </c>
-      <c r="H7" s="131">
+      <c r="H7" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="130">
+      <c r="I7" s="129">
         <v>0</v>
       </c>
-      <c r="J7" s="131">
+      <c r="J7" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="K7" s="130">
+      <c r="K7" s="129">
         <v>0</v>
       </c>
-      <c r="L7" s="131">
+      <c r="L7" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="M7" s="89"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="88"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="87"/>
     </row>
     <row r="8" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="146" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="85" t="s">
+      <c r="C8" s="82">
+        <v>62152074</v>
+      </c>
+      <c r="D8" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="130">
+      <c r="E8" s="129">
         <v>0</v>
       </c>
-      <c r="F8" s="131">
+      <c r="F8" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>130</v>
       </c>
-      <c r="G8" s="130">
+      <c r="G8" s="129">
         <v>2</v>
       </c>
-      <c r="H8" s="131">
+      <c r="H8" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="130">
+      <c r="I8" s="129">
         <v>0</v>
       </c>
-      <c r="J8" s="131">
+      <c r="J8" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="K8" s="130">
+      <c r="K8" s="129">
         <v>0</v>
       </c>
-      <c r="L8" s="131">
+      <c r="L8" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="M8" s="89"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="87"/>
     </row>
     <row r="9" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="144" t="s">
+      <c r="A9" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="145" t="s">
+      <c r="B9" s="138" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="146"/>
-      <c r="D9" s="147" t="s">
+      <c r="C9" s="139"/>
+      <c r="D9" s="140" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="130">
+      <c r="E9" s="129">
         <v>0</v>
       </c>
-      <c r="F9" s="131">
+      <c r="F9" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>102</v>
       </c>
-      <c r="G9" s="130">
+      <c r="G9" s="129">
         <v>3</v>
       </c>
-      <c r="H9" s="131">
+      <c r="H9" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="130">
+      <c r="I9" s="129">
         <v>0</v>
       </c>
-      <c r="J9" s="131">
+      <c r="J9" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="130">
+      <c r="K9" s="129">
         <v>0</v>
       </c>
-      <c r="L9" s="131">
+      <c r="L9" s="130">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="M9" s="89"/>
-      <c r="N9" s="87"/>
-      <c r="O9" s="89"/>
-      <c r="P9" s="88"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="149" t="s">
+      <c r="M9" s="88"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="87"/>
+    </row>
+    <row r="10" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="148" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="148"/>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="150">
+      <c r="B10" s="149"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="152">
         <f>SUM(E3:E9)*6</f>
         <v>0</v>
       </c>
-      <c r="F10" s="150">
+      <c r="F10" s="153">
         <f>RIGHT(E$1, (LEN(E$1)-FIND("_", E$1)))+RIGHT(E$1, (LEN(E$1)-FIND("_", E$1)))*0.3+RIGHT(E$1, (LEN(E$1)-FIND("_", E$1)))*0.65-E$10</f>
         <v>234</v>
       </c>
-      <c r="G10" s="150">
+      <c r="G10" s="152">
         <f>SUM(G3:G9)*6</f>
         <v>72</v>
       </c>
-      <c r="H10" s="150">
+      <c r="H10" s="153">
         <f>RIGHT(G$1, (LEN(G$1)-FIND("_", G$1)))*1+RIGHT(G$1, (LEN(G$1)-FIND("_", G$1)))*4*0.8+RIGHT(G$1, (LEN(G$1)-FIND("_", G$1)))*0.65-G$10</f>
         <v>655.5</v>
       </c>
-      <c r="I10" s="150">
+      <c r="I10" s="152">
         <f>SUM(I3:I9)*6</f>
         <v>0</v>
       </c>
-      <c r="J10" s="150">
+      <c r="J10" s="153">
         <f>RIGHT(I$1, (LEN(I$1)-FIND("_", I$1)))*6+RIGHT(I$1, (LEN(I$1)-FIND("_", I$1)))*0.65-I$10</f>
         <v>798</v>
       </c>
-      <c r="K10" s="150">
+      <c r="K10" s="152">
         <f>SUM(K3:K9)*6</f>
         <v>0</v>
       </c>
-      <c r="L10" s="150">
+      <c r="L10" s="153">
         <f>RIGHT(K$1, (LEN(K$1)-FIND("_", K$1)))*6+RIGHT(K$1, (LEN(K$1)-FIND("_", K$1)))*0.65-K$10</f>
         <v>798</v>
       </c>
-      <c r="M10" s="150"/>
-      <c r="N10" s="150">
+      <c r="M10" s="152"/>
+      <c r="N10" s="153">
         <f>RIGHT(M$1, (LEN(M$1)-FIND("_", M$1)))*6+RIGHT(M$1, (LEN(M$1)-FIND("_", M$1)))*0.65-M$10</f>
         <v>798</v>
       </c>
-      <c r="O10" s="150"/>
-      <c r="P10" s="150">
+      <c r="O10" s="152"/>
+      <c r="P10" s="153">
         <f>RIGHT(O$1, (LEN(O$1)-FIND("_", O$1)))*6+RIGHT(O$1, (LEN(O$1)-FIND("_", O$1)))*0.65-O$10</f>
         <v>798</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="129"/>
+      <c r="H17" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F3:F9 F11:F100">
-    <cfRule type="expression" dxfId="23" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>IF(AND(F3&gt;=(108-(E3*6)),F3&lt;(120-(E3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="30">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>IF(F3&gt;=(120 - E3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J9">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="23" priority="9">
       <formula>IF(AND(J3&gt;=(108-(I3*6)),J3&lt;(120-(I3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="10">
+    <cfRule type="expression" dxfId="22" priority="10">
       <formula>IF(J3&gt;=(120 - I3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L9">
-    <cfRule type="expression" dxfId="19" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>IF(AND(L3&gt;=(108-(K3*6)),L3&lt;(120-(K3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>IF(L3&gt;=(120 - K3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="17" priority="6">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>IF(F3&gt;=(120*0.65-(E3*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H9">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>IF(AND(H3&gt;=(108-(G3*6)),H3&lt;(120-(G3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>IF(H3&gt;=(120 - G3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>IF(H3&gt;=(120*0.65-(G3*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>IF(H4&gt;=(120*0.65-(G4*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>IF(H3&gt;=(120*0.65-(G3*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3524,16 +3564,16 @@
       <c r="A1" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="127" t="s">
+      <c r="C1" s="126" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="127" t="s">
+      <c r="D1" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="128" t="s">
+      <c r="E1" s="127" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3544,7 +3584,7 @@
       <c r="B2" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="132"/>
+      <c r="C2" s="131"/>
       <c r="D2" s="32" t="s">
         <v>16</v>
       </c>
@@ -3609,7 +3649,7 @@
       <c r="B7" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="133"/>
+      <c r="C7" s="132"/>
       <c r="D7" s="38" t="s">
         <v>64</v>
       </c>
@@ -3959,7 +3999,7 @@
     <row r="35" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="80"/>
       <c r="B35" s="81"/>
-      <c r="C35" s="134"/>
+      <c r="C35" s="133"/>
       <c r="D35" s="2"/>
       <c r="E35" s="3"/>
     </row>
@@ -4141,8 +4181,8 @@
       <c r="A50" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="101"/>
-      <c r="C50" s="101"/>
+      <c r="B50" s="100"/>
+      <c r="C50" s="100"/>
       <c r="D50" s="40" t="s">
         <v>19</v>
       </c>
@@ -4151,236 +4191,236 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="102" t="s">
+      <c r="A51" s="101" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="105" t="s">
+      <c r="B51" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="105"/>
-      <c r="D51" s="106" t="s">
+      <c r="C51" s="104"/>
+      <c r="D51" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="E51" s="107">
+      <c r="E51" s="106">
         <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="103"/>
-      <c r="B52" s="108" t="s">
+      <c r="A52" s="102"/>
+      <c r="B52" s="107" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="108"/>
-      <c r="D52" s="109" t="s">
+      <c r="C52" s="107"/>
+      <c r="D52" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="E52" s="110">
+      <c r="E52" s="109">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="103"/>
-      <c r="B53" s="108" t="s">
+      <c r="A53" s="102"/>
+      <c r="B53" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="C53" s="108"/>
-      <c r="D53" s="109" t="s">
+      <c r="C53" s="107"/>
+      <c r="D53" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="E53" s="110">
+      <c r="E53" s="109">
         <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="103"/>
-      <c r="B54" s="108" t="s">
+      <c r="A54" s="102"/>
+      <c r="B54" s="107" t="s">
         <v>129</v>
       </c>
-      <c r="C54" s="108"/>
-      <c r="D54" s="109" t="s">
+      <c r="C54" s="107"/>
+      <c r="D54" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="E54" s="110">
+      <c r="E54" s="109">
         <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="103"/>
-      <c r="B55" s="108" t="s">
+      <c r="A55" s="102"/>
+      <c r="B55" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="C55" s="108"/>
-      <c r="D55" s="109" t="s">
+      <c r="C55" s="107"/>
+      <c r="D55" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="E55" s="110">
+      <c r="E55" s="109">
         <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="103"/>
-      <c r="B56" s="108" t="s">
+      <c r="A56" s="102"/>
+      <c r="B56" s="107" t="s">
         <v>131</v>
       </c>
-      <c r="C56" s="108"/>
-      <c r="D56" s="109" t="s">
+      <c r="C56" s="107"/>
+      <c r="D56" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="E56" s="110">
+      <c r="E56" s="109">
         <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="103"/>
-      <c r="B57" s="108" t="s">
+      <c r="A57" s="102"/>
+      <c r="B57" s="107" t="s">
         <v>132</v>
       </c>
-      <c r="C57" s="108"/>
-      <c r="D57" s="109" t="s">
+      <c r="C57" s="107"/>
+      <c r="D57" s="108" t="s">
         <v>124</v>
       </c>
-      <c r="E57" s="110">
+      <c r="E57" s="109">
         <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="103"/>
-      <c r="B58" s="108" t="s">
+      <c r="A58" s="102"/>
+      <c r="B58" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="C58" s="108"/>
-      <c r="D58" s="109" t="s">
+      <c r="C58" s="107"/>
+      <c r="D58" s="108" t="s">
         <v>124</v>
       </c>
-      <c r="E58" s="110">
+      <c r="E58" s="109">
         <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="103"/>
-      <c r="B59" s="108" t="s">
+      <c r="A59" s="102"/>
+      <c r="B59" s="107" t="s">
         <v>134</v>
       </c>
-      <c r="C59" s="108"/>
-      <c r="D59" s="109" t="s">
+      <c r="C59" s="107"/>
+      <c r="D59" s="108" t="s">
         <v>125</v>
       </c>
-      <c r="E59" s="110">
+      <c r="E59" s="109">
         <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="103"/>
-      <c r="B60" s="108" t="s">
+      <c r="A60" s="102"/>
+      <c r="B60" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="C60" s="108"/>
-      <c r="D60" s="109" t="s">
+      <c r="C60" s="107"/>
+      <c r="D60" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="E60" s="110">
+      <c r="E60" s="109">
         <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="103"/>
-      <c r="B61" s="108" t="s">
+      <c r="A61" s="102"/>
+      <c r="B61" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="C61" s="108"/>
-      <c r="D61" s="109" t="s">
+      <c r="C61" s="107"/>
+      <c r="D61" s="108" t="s">
         <v>125</v>
       </c>
-      <c r="E61" s="110">
+      <c r="E61" s="109">
         <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="104"/>
-      <c r="B62" s="111" t="s">
+      <c r="A62" s="103"/>
+      <c r="B62" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="111"/>
-      <c r="D62" s="112" t="s">
+      <c r="C62" s="110"/>
+      <c r="D62" s="111" t="s">
         <v>127</v>
       </c>
-      <c r="E62" s="113">
+      <c r="E62" s="112">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="60"/>
-      <c r="B63" s="114" t="s">
+      <c r="B63" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="114"/>
-      <c r="D63" s="115"/>
-      <c r="E63" s="116"/>
+      <c r="C63" s="113"/>
+      <c r="D63" s="114"/>
+      <c r="E63" s="115"/>
     </row>
     <row r="64" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="62"/>
-      <c r="B64" s="117" t="s">
+      <c r="B64" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="117"/>
-      <c r="D64" s="118"/>
-      <c r="E64" s="119"/>
+      <c r="C64" s="116"/>
+      <c r="D64" s="117"/>
+      <c r="E64" s="118"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="61"/>
-      <c r="B65" s="120" t="s">
+      <c r="B65" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="C65" s="120"/>
-      <c r="D65" s="121"/>
-      <c r="E65" s="122"/>
+      <c r="C65" s="119"/>
+      <c r="D65" s="120"/>
+      <c r="E65" s="121"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="123" t="s">
+      <c r="B66" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="C66" s="123"/>
-      <c r="D66" s="124"/>
-      <c r="E66" s="125"/>
+      <c r="C66" s="122"/>
+      <c r="D66" s="123"/>
+      <c r="E66" s="124"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="62"/>
-      <c r="B67" s="123" t="s">
+      <c r="B67" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="C67" s="123"/>
-      <c r="D67" s="124"/>
-      <c r="E67" s="125"/>
+      <c r="C67" s="122"/>
+      <c r="D67" s="123"/>
+      <c r="E67" s="124"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="62"/>
-      <c r="B68" s="123" t="s">
+      <c r="B68" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="C68" s="135"/>
-      <c r="D68" s="126"/>
-      <c r="E68" s="125"/>
+      <c r="C68" s="134"/>
+      <c r="D68" s="125"/>
+      <c r="E68" s="124"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="62"/>
-      <c r="B69" s="123" t="s">
+      <c r="B69" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="123"/>
-      <c r="D69" s="124"/>
-      <c r="E69" s="125"/>
+      <c r="C69" s="122"/>
+      <c r="D69" s="123"/>
+      <c r="E69" s="124"/>
     </row>
     <row r="70" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="63"/>
-      <c r="B70" s="117" t="s">
+      <c r="B70" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="C70" s="117"/>
-      <c r="D70" s="118"/>
-      <c r="E70" s="119"/>
+      <c r="C70" s="116"/>
+      <c r="D70" s="117"/>
+      <c r="E70" s="118"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -4530,547 +4570,547 @@
       <c r="A1" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="127" t="s">
+      <c r="C1" s="126" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="135" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="128" t="s">
+      <c r="E1" s="127" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="94"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="93"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96" t="s">
+      <c r="A3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="97"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="95"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="97"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="96"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="97"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="95"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="97"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="95"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="97"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="96"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="95"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="96"/>
     </row>
     <row r="10" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="100"/>
+      <c r="A10" s="97"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="99"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="94"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="93"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="95"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="97"/>
+      <c r="A12" s="94"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="96"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="96"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="97"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="96"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="95"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="97"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="97"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="97"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="97"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="96"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="98"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="100"/>
+      <c r="A20" s="97"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="99"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
-      <c r="E21" s="94"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="93"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="97"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="95"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
+      <c r="A23" s="94"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="95"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="97"/>
+      <c r="A24" s="94"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="96"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="97"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="96"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="95"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="97"/>
+      <c r="A26" s="94"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="96"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="95"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
+      <c r="A27" s="94"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="96"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="97"/>
+      <c r="A28" s="94"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="97"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="96"/>
     </row>
     <row r="30" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="98"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="100"/>
+      <c r="A30" s="97"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="99"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="93" t="s">
+      <c r="A31" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="94"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="93"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="97"/>
+      <c r="A32" s="94"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="96"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="95"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="97"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="96"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="96"/>
-      <c r="D34" s="96"/>
-      <c r="E34" s="97"/>
+      <c r="A34" s="94"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="96"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="95"/>
-      <c r="B35" s="96"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="97"/>
+      <c r="A35" s="94"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="96"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="95"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="96"/>
-      <c r="D36" s="96"/>
-      <c r="E36" s="97"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="96"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="95"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="97"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="96"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="95"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="97"/>
+      <c r="A38" s="94"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="95"/>
+      <c r="E38" s="96"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="95"/>
-      <c r="B39" s="96"/>
-      <c r="C39" s="96"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="97"/>
+      <c r="A39" s="94"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="96"/>
     </row>
     <row r="40" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="98"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="100"/>
+      <c r="A40" s="97"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="99"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="94"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="91"/>
+      <c r="E41" s="93"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="95"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="97"/>
+      <c r="A42" s="94"/>
+      <c r="B42" s="95"/>
+      <c r="C42" s="95"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="96"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="95"/>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="97"/>
+      <c r="A43" s="94"/>
+      <c r="B43" s="95"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="96"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="95"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="96"/>
-      <c r="D44" s="96"/>
-      <c r="E44" s="97"/>
+      <c r="A44" s="94"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="96"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="95"/>
-      <c r="B45" s="96"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="96"/>
-      <c r="E45" s="97"/>
+      <c r="A45" s="94"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="95"/>
+      <c r="E45" s="96"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="95"/>
-      <c r="B46" s="96"/>
-      <c r="C46" s="96"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="97"/>
+      <c r="A46" s="94"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="96"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="95"/>
-      <c r="B47" s="96"/>
-      <c r="C47" s="96"/>
-      <c r="D47" s="96"/>
-      <c r="E47" s="97"/>
+      <c r="A47" s="94"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="96"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="95"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="96"/>
-      <c r="D48" s="96"/>
-      <c r="E48" s="97"/>
+      <c r="A48" s="94"/>
+      <c r="B48" s="95"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="96"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="95"/>
-      <c r="B49" s="96"/>
-      <c r="C49" s="96"/>
-      <c r="D49" s="96"/>
-      <c r="E49" s="97"/>
+      <c r="A49" s="94"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="96"/>
     </row>
     <row r="50" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="98"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="100"/>
+      <c r="A50" s="97"/>
+      <c r="B50" s="98"/>
+      <c r="C50" s="98"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="99"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="92"/>
-      <c r="C51" s="92"/>
-      <c r="D51" s="92"/>
-      <c r="E51" s="94"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="93"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="95"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="96"/>
-      <c r="D52" s="96"/>
-      <c r="E52" s="97"/>
+      <c r="A52" s="94"/>
+      <c r="B52" s="95"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="96"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="95"/>
-      <c r="B53" s="96"/>
-      <c r="C53" s="96"/>
-      <c r="D53" s="96"/>
-      <c r="E53" s="97"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="96"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="95"/>
-      <c r="B54" s="96"/>
-      <c r="C54" s="96"/>
-      <c r="D54" s="96"/>
-      <c r="E54" s="97"/>
+      <c r="A54" s="94"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="96"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="95"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="96"/>
-      <c r="D55" s="96"/>
-      <c r="E55" s="97"/>
+      <c r="A55" s="94"/>
+      <c r="B55" s="95"/>
+      <c r="C55" s="95"/>
+      <c r="D55" s="95"/>
+      <c r="E55" s="96"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="95"/>
-      <c r="B56" s="96"/>
-      <c r="C56" s="96"/>
-      <c r="D56" s="96"/>
-      <c r="E56" s="97"/>
+      <c r="A56" s="94"/>
+      <c r="B56" s="95"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="95"/>
+      <c r="E56" s="96"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="95"/>
-      <c r="B57" s="96"/>
-      <c r="C57" s="96"/>
-      <c r="D57" s="96"/>
-      <c r="E57" s="97"/>
+      <c r="A57" s="94"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="96"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="95"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="96"/>
-      <c r="D58" s="96"/>
-      <c r="E58" s="97"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="96"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="95"/>
-      <c r="B59" s="96"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="96"/>
-      <c r="E59" s="97"/>
+      <c r="A59" s="94"/>
+      <c r="B59" s="95"/>
+      <c r="C59" s="95"/>
+      <c r="D59" s="95"/>
+      <c r="E59" s="96"/>
     </row>
     <row r="60" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="98"/>
-      <c r="B60" s="99"/>
-      <c r="C60" s="99"/>
-      <c r="D60" s="99"/>
-      <c r="E60" s="100"/>
+      <c r="A60" s="97"/>
+      <c r="B60" s="98"/>
+      <c r="C60" s="98"/>
+      <c r="D60" s="98"/>
+      <c r="E60" s="99"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="93" t="s">
+      <c r="A61" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="92"/>
-      <c r="C61" s="92"/>
-      <c r="D61" s="92"/>
-      <c r="E61" s="94"/>
+      <c r="B61" s="91"/>
+      <c r="C61" s="91"/>
+      <c r="D61" s="91"/>
+      <c r="E61" s="93"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="95"/>
-      <c r="B62" s="96"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="97"/>
+      <c r="A62" s="94"/>
+      <c r="B62" s="95"/>
+      <c r="C62" s="95"/>
+      <c r="D62" s="95"/>
+      <c r="E62" s="96"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="95"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="96"/>
-      <c r="D63" s="96"/>
-      <c r="E63" s="97"/>
+      <c r="A63" s="94"/>
+      <c r="B63" s="95"/>
+      <c r="C63" s="95"/>
+      <c r="D63" s="95"/>
+      <c r="E63" s="96"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="95"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="96"/>
-      <c r="D64" s="96"/>
-      <c r="E64" s="97"/>
+      <c r="A64" s="94"/>
+      <c r="B64" s="95"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="95"/>
+      <c r="E64" s="96"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="95"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="96"/>
-      <c r="E65" s="97"/>
+      <c r="A65" s="94"/>
+      <c r="B65" s="95"/>
+      <c r="C65" s="95"/>
+      <c r="D65" s="95"/>
+      <c r="E65" s="96"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="95"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="96"/>
-      <c r="E66" s="97"/>
+      <c r="A66" s="94"/>
+      <c r="B66" s="95"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="96"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="95"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="96"/>
-      <c r="E67" s="97"/>
+      <c r="A67" s="94"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="95"/>
+      <c r="D67" s="95"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="95"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="96"/>
-      <c r="D68" s="96"/>
-      <c r="E68" s="97"/>
+      <c r="A68" s="94"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="95"/>
+      <c r="D68" s="95"/>
+      <c r="E68" s="96"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="95"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="96"/>
-      <c r="E69" s="97"/>
+      <c r="A69" s="94"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="95"/>
+      <c r="E69" s="96"/>
     </row>
     <row r="70" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="98"/>
-      <c r="B70" s="99"/>
-      <c r="C70" s="99"/>
-      <c r="D70" s="99"/>
-      <c r="E70" s="100"/>
+      <c r="A70" s="97"/>
+      <c r="B70" s="98"/>
+      <c r="C70" s="98"/>
+      <c r="D70" s="98"/>
+      <c r="E70" s="99"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="93" t="s">
+      <c r="A71" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="92"/>
-      <c r="C71" s="92"/>
-      <c r="D71" s="92"/>
-      <c r="E71" s="94"/>
+      <c r="B71" s="91"/>
+      <c r="C71" s="91"/>
+      <c r="D71" s="91"/>
+      <c r="E71" s="93"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="95"/>
-      <c r="B72" s="96"/>
-      <c r="C72" s="96"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="97"/>
+      <c r="A72" s="94"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="95"/>
+      <c r="E72" s="96"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="95"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="96"/>
-      <c r="D73" s="96"/>
-      <c r="E73" s="97"/>
+      <c r="A73" s="94"/>
+      <c r="B73" s="95"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="96"/>
     </row>
     <row r="74" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="98"/>
-      <c r="B74" s="99"/>
-      <c r="C74" s="99"/>
-      <c r="D74" s="99"/>
-      <c r="E74" s="100"/>
+      <c r="A74" s="97"/>
+      <c r="B74" s="98"/>
+      <c r="C74" s="98"/>
+      <c r="D74" s="98"/>
+      <c r="E74" s="99"/>
     </row>
     <row r="75" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="58" t="s">
@@ -5078,7 +5118,7 @@
       </c>
       <c r="B75" s="57"/>
       <c r="C75" s="16"/>
-      <c r="D75" s="137"/>
+      <c r="D75" s="136"/>
       <c r="E75" s="17">
         <v>0</v>
       </c>
@@ -5089,7 +5129,7 @@
       </c>
       <c r="B76" s="59"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="138"/>
+      <c r="D76" s="137"/>
       <c r="E76" s="3">
         <v>0</v>
       </c>
@@ -5097,22 +5137,22 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I56:I57">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H58">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F58">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>IF(#REF!=1, 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E100">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>IF($C2=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5151,545 +5191,545 @@
       <c r="A1" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="127" t="s">
+      <c r="C1" s="126" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="135" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="128" t="s">
+      <c r="E1" s="127" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="94"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="93"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="97"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="95"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="97"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="96"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="97"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="95"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="97"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="95"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="97"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="96"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="95"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="96"/>
     </row>
     <row r="10" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="100"/>
+      <c r="A10" s="97"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="99"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="94"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="93"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="95"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="97"/>
+      <c r="A12" s="94"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="96"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="96"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="97"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="96"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="95"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="97"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="97"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="97"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="97"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="96"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="98"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="100"/>
+      <c r="A20" s="97"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="99"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
-      <c r="E21" s="94"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="93"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="97"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="95"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
+      <c r="A23" s="94"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="95"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="97"/>
+      <c r="A24" s="94"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="96"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="97"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="96"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="95"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="97"/>
+      <c r="A26" s="94"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="96"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="95"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
+      <c r="A27" s="94"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="96"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="97"/>
+      <c r="A28" s="94"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="97"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="96"/>
     </row>
     <row r="30" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="98"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="100"/>
+      <c r="A30" s="97"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="99"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="93" t="s">
+      <c r="A31" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="94"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="93"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="97"/>
+      <c r="A32" s="94"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="96"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="95"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="97"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="96"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="96"/>
-      <c r="D34" s="96"/>
-      <c r="E34" s="97"/>
+      <c r="A34" s="94"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="96"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="95"/>
-      <c r="B35" s="96"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="97"/>
+      <c r="A35" s="94"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="96"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="95"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="96"/>
-      <c r="D36" s="96"/>
-      <c r="E36" s="97"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="96"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="95"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="97"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="96"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="95"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="97"/>
+      <c r="A38" s="94"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="95"/>
+      <c r="E38" s="96"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="95"/>
-      <c r="B39" s="96"/>
-      <c r="C39" s="96"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="97"/>
+      <c r="A39" s="94"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="96"/>
     </row>
     <row r="40" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="98"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="100"/>
+      <c r="A40" s="97"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="99"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="94"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="91"/>
+      <c r="E41" s="93"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="95"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="97"/>
+      <c r="A42" s="94"/>
+      <c r="B42" s="95"/>
+      <c r="C42" s="95"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="96"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="95"/>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="97"/>
+      <c r="A43" s="94"/>
+      <c r="B43" s="95"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="96"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="95"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="96"/>
-      <c r="D44" s="96"/>
-      <c r="E44" s="97"/>
+      <c r="A44" s="94"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="96"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="95"/>
-      <c r="B45" s="96"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="96"/>
-      <c r="E45" s="97"/>
+      <c r="A45" s="94"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="95"/>
+      <c r="E45" s="96"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="95"/>
-      <c r="B46" s="96"/>
-      <c r="C46" s="96"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="97"/>
+      <c r="A46" s="94"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="96"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="95"/>
-      <c r="B47" s="96"/>
-      <c r="C47" s="96"/>
-      <c r="D47" s="96"/>
-      <c r="E47" s="97"/>
+      <c r="A47" s="94"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="96"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="95"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="96"/>
-      <c r="D48" s="96"/>
-      <c r="E48" s="97"/>
+      <c r="A48" s="94"/>
+      <c r="B48" s="95"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="96"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="95"/>
-      <c r="B49" s="96"/>
-      <c r="C49" s="96"/>
-      <c r="D49" s="96"/>
-      <c r="E49" s="97"/>
+      <c r="A49" s="94"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="96"/>
     </row>
     <row r="50" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="98"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="100"/>
+      <c r="A50" s="97"/>
+      <c r="B50" s="98"/>
+      <c r="C50" s="98"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="99"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="92"/>
-      <c r="C51" s="92"/>
-      <c r="D51" s="92"/>
-      <c r="E51" s="94"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="93"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="95"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="96"/>
-      <c r="D52" s="96"/>
-      <c r="E52" s="97"/>
+      <c r="A52" s="94"/>
+      <c r="B52" s="95"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="96"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="95"/>
-      <c r="B53" s="96"/>
-      <c r="C53" s="96"/>
-      <c r="D53" s="96"/>
-      <c r="E53" s="97"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="96"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="95"/>
-      <c r="B54" s="96"/>
-      <c r="C54" s="96"/>
-      <c r="D54" s="96"/>
-      <c r="E54" s="97"/>
+      <c r="A54" s="94"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="96"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="95"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="96"/>
-      <c r="D55" s="96"/>
-      <c r="E55" s="97"/>
+      <c r="A55" s="94"/>
+      <c r="B55" s="95"/>
+      <c r="C55" s="95"/>
+      <c r="D55" s="95"/>
+      <c r="E55" s="96"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="95"/>
-      <c r="B56" s="96"/>
-      <c r="C56" s="96"/>
-      <c r="D56" s="96"/>
-      <c r="E56" s="97"/>
+      <c r="A56" s="94"/>
+      <c r="B56" s="95"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="95"/>
+      <c r="E56" s="96"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="95"/>
-      <c r="B57" s="96"/>
-      <c r="C57" s="96"/>
-      <c r="D57" s="96"/>
-      <c r="E57" s="97"/>
+      <c r="A57" s="94"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="96"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="95"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="96"/>
-      <c r="D58" s="96"/>
-      <c r="E58" s="97"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="96"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="95"/>
-      <c r="B59" s="96"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="96"/>
-      <c r="E59" s="97"/>
+      <c r="A59" s="94"/>
+      <c r="B59" s="95"/>
+      <c r="C59" s="95"/>
+      <c r="D59" s="95"/>
+      <c r="E59" s="96"/>
     </row>
     <row r="60" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="98"/>
-      <c r="B60" s="99"/>
-      <c r="C60" s="99"/>
-      <c r="D60" s="99"/>
-      <c r="E60" s="100"/>
+      <c r="A60" s="97"/>
+      <c r="B60" s="98"/>
+      <c r="C60" s="98"/>
+      <c r="D60" s="98"/>
+      <c r="E60" s="99"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="93" t="s">
+      <c r="A61" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="92"/>
-      <c r="C61" s="92"/>
-      <c r="D61" s="92"/>
-      <c r="E61" s="94"/>
+      <c r="B61" s="91"/>
+      <c r="C61" s="91"/>
+      <c r="D61" s="91"/>
+      <c r="E61" s="93"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="95"/>
-      <c r="B62" s="96"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="97"/>
+      <c r="A62" s="94"/>
+      <c r="B62" s="95"/>
+      <c r="C62" s="95"/>
+      <c r="D62" s="95"/>
+      <c r="E62" s="96"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="95"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="96"/>
-      <c r="D63" s="96"/>
-      <c r="E63" s="97"/>
+      <c r="A63" s="94"/>
+      <c r="B63" s="95"/>
+      <c r="C63" s="95"/>
+      <c r="D63" s="95"/>
+      <c r="E63" s="96"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="95"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="96"/>
-      <c r="D64" s="96"/>
-      <c r="E64" s="97"/>
+      <c r="A64" s="94"/>
+      <c r="B64" s="95"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="95"/>
+      <c r="E64" s="96"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="95"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="96"/>
-      <c r="E65" s="97"/>
+      <c r="A65" s="94"/>
+      <c r="B65" s="95"/>
+      <c r="C65" s="95"/>
+      <c r="D65" s="95"/>
+      <c r="E65" s="96"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="95"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="96"/>
-      <c r="E66" s="97"/>
+      <c r="A66" s="94"/>
+      <c r="B66" s="95"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="96"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="95"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="96"/>
-      <c r="E67" s="97"/>
+      <c r="A67" s="94"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="95"/>
+      <c r="D67" s="95"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="95"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="96"/>
-      <c r="D68" s="96"/>
-      <c r="E68" s="97"/>
+      <c r="A68" s="94"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="95"/>
+      <c r="D68" s="95"/>
+      <c r="E68" s="96"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="95"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="96"/>
-      <c r="E69" s="97"/>
+      <c r="A69" s="94"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="95"/>
+      <c r="E69" s="96"/>
     </row>
     <row r="70" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="98"/>
-      <c r="B70" s="99"/>
-      <c r="C70" s="99"/>
-      <c r="D70" s="99"/>
-      <c r="E70" s="100"/>
+      <c r="A70" s="97"/>
+      <c r="B70" s="98"/>
+      <c r="C70" s="98"/>
+      <c r="D70" s="98"/>
+      <c r="E70" s="99"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="93" t="s">
+      <c r="A71" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="92"/>
-      <c r="C71" s="92"/>
-      <c r="D71" s="92"/>
-      <c r="E71" s="94"/>
+      <c r="B71" s="91"/>
+      <c r="C71" s="91"/>
+      <c r="D71" s="91"/>
+      <c r="E71" s="93"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="95"/>
-      <c r="B72" s="96"/>
-      <c r="C72" s="96"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="97"/>
+      <c r="A72" s="94"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="95"/>
+      <c r="E72" s="96"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="95"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="96"/>
-      <c r="D73" s="96"/>
-      <c r="E73" s="97"/>
+      <c r="A73" s="94"/>
+      <c r="B73" s="95"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="96"/>
     </row>
     <row r="74" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="98"/>
-      <c r="B74" s="99"/>
-      <c r="C74" s="99"/>
-      <c r="D74" s="99"/>
-      <c r="E74" s="100"/>
+      <c r="A74" s="97"/>
+      <c r="B74" s="98"/>
+      <c r="C74" s="98"/>
+      <c r="D74" s="98"/>
+      <c r="E74" s="99"/>
     </row>
     <row r="75" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="58" t="s">
@@ -5697,7 +5737,7 @@
       </c>
       <c r="B75" s="57"/>
       <c r="C75" s="16"/>
-      <c r="D75" s="137"/>
+      <c r="D75" s="136"/>
       <c r="E75" s="17">
         <v>0</v>
       </c>
@@ -5708,7 +5748,7 @@
       </c>
       <c r="B76" s="59"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="138"/>
+      <c r="D76" s="137"/>
       <c r="E76" s="3">
         <v>0</v>
       </c>
@@ -5716,22 +5756,22 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I56:I57">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H58">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F58">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>IF(#REF!=1, 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E100">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>IF($C2=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5771,545 +5811,545 @@
       <c r="A1" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="127" t="s">
+      <c r="C1" s="126" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="135" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="128" t="s">
+      <c r="E1" s="127" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="94"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="93"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="97"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="96"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="95"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="97"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="96"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="97"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="95"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="97"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="95"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="97"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="96"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="95"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="96"/>
     </row>
     <row r="10" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="100"/>
+      <c r="A10" s="97"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="99"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="94"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="93"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="95"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="97"/>
+      <c r="A12" s="94"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="96"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="96"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="97"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="96"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="95"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="97"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="97"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="97"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="97"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="96"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="98"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="100"/>
+      <c r="A20" s="97"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="99"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
-      <c r="E21" s="94"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="93"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="97"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="95"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
+      <c r="A23" s="94"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="95"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="97"/>
+      <c r="A24" s="94"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="96"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="97"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="96"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="95"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="97"/>
+      <c r="A26" s="94"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="96"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="95"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97"/>
+      <c r="A27" s="94"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="96"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="97"/>
+      <c r="A28" s="94"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="97"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="96"/>
     </row>
     <row r="30" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="98"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="100"/>
+      <c r="A30" s="97"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="99"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="93" t="s">
+      <c r="A31" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="94"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="93"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="97"/>
+      <c r="A32" s="94"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="96"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="95"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="97"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="96"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="96"/>
-      <c r="D34" s="96"/>
-      <c r="E34" s="97"/>
+      <c r="A34" s="94"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="96"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="95"/>
-      <c r="B35" s="96"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="97"/>
+      <c r="A35" s="94"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="96"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="95"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="96"/>
-      <c r="D36" s="96"/>
-      <c r="E36" s="97"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="96"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="95"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="97"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="96"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="95"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="97"/>
+      <c r="A38" s="94"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="95"/>
+      <c r="E38" s="96"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="95"/>
-      <c r="B39" s="96"/>
-      <c r="C39" s="96"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="97"/>
+      <c r="A39" s="94"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="96"/>
     </row>
     <row r="40" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="98"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="100"/>
+      <c r="A40" s="97"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="99"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="94"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="91"/>
+      <c r="E41" s="93"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="95"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="97"/>
+      <c r="A42" s="94"/>
+      <c r="B42" s="95"/>
+      <c r="C42" s="95"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="96"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="95"/>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="97"/>
+      <c r="A43" s="94"/>
+      <c r="B43" s="95"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="96"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="95"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="96"/>
-      <c r="D44" s="96"/>
-      <c r="E44" s="97"/>
+      <c r="A44" s="94"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="96"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="95"/>
-      <c r="B45" s="96"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="96"/>
-      <c r="E45" s="97"/>
+      <c r="A45" s="94"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="95"/>
+      <c r="E45" s="96"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="95"/>
-      <c r="B46" s="96"/>
-      <c r="C46" s="96"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="97"/>
+      <c r="A46" s="94"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="96"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="95"/>
-      <c r="B47" s="96"/>
-      <c r="C47" s="96"/>
-      <c r="D47" s="96"/>
-      <c r="E47" s="97"/>
+      <c r="A47" s="94"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="96"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="95"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="96"/>
-      <c r="D48" s="96"/>
-      <c r="E48" s="97"/>
+      <c r="A48" s="94"/>
+      <c r="B48" s="95"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="96"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="95"/>
-      <c r="B49" s="96"/>
-      <c r="C49" s="96"/>
-      <c r="D49" s="96"/>
-      <c r="E49" s="97"/>
+      <c r="A49" s="94"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="96"/>
     </row>
     <row r="50" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="98"/>
-      <c r="B50" s="99"/>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="100"/>
+      <c r="A50" s="97"/>
+      <c r="B50" s="98"/>
+      <c r="C50" s="98"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="99"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="93" t="s">
+      <c r="A51" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="92"/>
-      <c r="C51" s="92"/>
-      <c r="D51" s="92"/>
-      <c r="E51" s="94"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="93"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="95"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="96"/>
-      <c r="D52" s="96"/>
-      <c r="E52" s="97"/>
+      <c r="A52" s="94"/>
+      <c r="B52" s="95"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="96"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="95"/>
-      <c r="B53" s="96"/>
-      <c r="C53" s="96"/>
-      <c r="D53" s="96"/>
-      <c r="E53" s="97"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="96"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="95"/>
-      <c r="B54" s="96"/>
-      <c r="C54" s="96"/>
-      <c r="D54" s="96"/>
-      <c r="E54" s="97"/>
+      <c r="A54" s="94"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="96"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="95"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="96"/>
-      <c r="D55" s="96"/>
-      <c r="E55" s="97"/>
+      <c r="A55" s="94"/>
+      <c r="B55" s="95"/>
+      <c r="C55" s="95"/>
+      <c r="D55" s="95"/>
+      <c r="E55" s="96"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="95"/>
-      <c r="B56" s="96"/>
-      <c r="C56" s="96"/>
-      <c r="D56" s="96"/>
-      <c r="E56" s="97"/>
+      <c r="A56" s="94"/>
+      <c r="B56" s="95"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="95"/>
+      <c r="E56" s="96"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="95"/>
-      <c r="B57" s="96"/>
-      <c r="C57" s="96"/>
-      <c r="D57" s="96"/>
-      <c r="E57" s="97"/>
+      <c r="A57" s="94"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="95"/>
+      <c r="E57" s="96"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="95"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="96"/>
-      <c r="D58" s="96"/>
-      <c r="E58" s="97"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="96"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="95"/>
-      <c r="B59" s="96"/>
-      <c r="C59" s="96"/>
-      <c r="D59" s="96"/>
-      <c r="E59" s="97"/>
+      <c r="A59" s="94"/>
+      <c r="B59" s="95"/>
+      <c r="C59" s="95"/>
+      <c r="D59" s="95"/>
+      <c r="E59" s="96"/>
     </row>
     <row r="60" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="98"/>
-      <c r="B60" s="99"/>
-      <c r="C60" s="99"/>
-      <c r="D60" s="99"/>
-      <c r="E60" s="100"/>
+      <c r="A60" s="97"/>
+      <c r="B60" s="98"/>
+      <c r="C60" s="98"/>
+      <c r="D60" s="98"/>
+      <c r="E60" s="99"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="93" t="s">
+      <c r="A61" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B61" s="92"/>
-      <c r="C61" s="92"/>
-      <c r="D61" s="92"/>
-      <c r="E61" s="94"/>
+      <c r="B61" s="91"/>
+      <c r="C61" s="91"/>
+      <c r="D61" s="91"/>
+      <c r="E61" s="93"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="95"/>
-      <c r="B62" s="96"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="97"/>
+      <c r="A62" s="94"/>
+      <c r="B62" s="95"/>
+      <c r="C62" s="95"/>
+      <c r="D62" s="95"/>
+      <c r="E62" s="96"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="95"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="96"/>
-      <c r="D63" s="96"/>
-      <c r="E63" s="97"/>
+      <c r="A63" s="94"/>
+      <c r="B63" s="95"/>
+      <c r="C63" s="95"/>
+      <c r="D63" s="95"/>
+      <c r="E63" s="96"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="95"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="96"/>
-      <c r="D64" s="96"/>
-      <c r="E64" s="97"/>
+      <c r="A64" s="94"/>
+      <c r="B64" s="95"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="95"/>
+      <c r="E64" s="96"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="95"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="96"/>
-      <c r="D65" s="96"/>
-      <c r="E65" s="97"/>
+      <c r="A65" s="94"/>
+      <c r="B65" s="95"/>
+      <c r="C65" s="95"/>
+      <c r="D65" s="95"/>
+      <c r="E65" s="96"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="95"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="96"/>
-      <c r="D66" s="96"/>
-      <c r="E66" s="97"/>
+      <c r="A66" s="94"/>
+      <c r="B66" s="95"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="96"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="95"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="96"/>
-      <c r="E67" s="97"/>
+      <c r="A67" s="94"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="95"/>
+      <c r="D67" s="95"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="95"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="96"/>
-      <c r="D68" s="96"/>
-      <c r="E68" s="97"/>
+      <c r="A68" s="94"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="95"/>
+      <c r="D68" s="95"/>
+      <c r="E68" s="96"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="95"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="96"/>
-      <c r="E69" s="97"/>
+      <c r="A69" s="94"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="95"/>
+      <c r="E69" s="96"/>
     </row>
     <row r="70" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="98"/>
-      <c r="B70" s="99"/>
-      <c r="C70" s="99"/>
-      <c r="D70" s="99"/>
-      <c r="E70" s="100"/>
+      <c r="A70" s="97"/>
+      <c r="B70" s="98"/>
+      <c r="C70" s="98"/>
+      <c r="D70" s="98"/>
+      <c r="E70" s="99"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="93" t="s">
+      <c r="A71" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="92"/>
-      <c r="C71" s="92"/>
-      <c r="D71" s="92"/>
-      <c r="E71" s="94"/>
+      <c r="B71" s="91"/>
+      <c r="C71" s="91"/>
+      <c r="D71" s="91"/>
+      <c r="E71" s="93"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="95"/>
-      <c r="B72" s="96"/>
-      <c r="C72" s="96"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="97"/>
+      <c r="A72" s="94"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="95"/>
+      <c r="E72" s="96"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="95"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="96"/>
-      <c r="D73" s="96"/>
-      <c r="E73" s="97"/>
+      <c r="A73" s="94"/>
+      <c r="B73" s="95"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="96"/>
     </row>
     <row r="74" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="98"/>
-      <c r="B74" s="99"/>
-      <c r="C74" s="99"/>
-      <c r="D74" s="99"/>
-      <c r="E74" s="100"/>
+      <c r="A74" s="97"/>
+      <c r="B74" s="98"/>
+      <c r="C74" s="98"/>
+      <c r="D74" s="98"/>
+      <c r="E74" s="99"/>
     </row>
     <row r="75" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="58" t="s">
@@ -6317,7 +6357,7 @@
       </c>
       <c r="B75" s="57"/>
       <c r="C75" s="16"/>
-      <c r="D75" s="137"/>
+      <c r="D75" s="136"/>
       <c r="E75" s="17">
         <v>0</v>
       </c>
@@ -6328,7 +6368,7 @@
       </c>
       <c r="B76" s="59"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="138"/>
+      <c r="D76" s="137"/>
       <c r="E76" s="3">
         <v>0</v>
       </c>
@@ -6336,22 +6376,22 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I56:I57">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H58">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F58">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>IF(#REF!=1, 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E100">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF($C2=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add tlh nokia id info
</commit_message>
<xml_diff>
--- a/01_FBs_Plan.xlsx
+++ b/01_FBs_Plan.xlsx
@@ -2073,43 +2073,43 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="59" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="60" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="59" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="60" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2117,26 +2117,55 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="40">
     <dxf>
-      <font>
-        <color rgb="FFBA40A9"/>
-      </font>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <name val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.59999389629810485"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2156,96 +2185,6 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFBA40A9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
       </font>
     </dxf>
     <dxf>
@@ -2298,6 +2237,26 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFBA40A9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="medium">
           <color indexed="64"/>
@@ -2347,53 +2306,24 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <font>
+        <color rgb="FFBA40A9"/>
+      </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <name val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
+        <color rgb="FFFF0000"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6" tint="0.59999389629810485"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2606,6 +2536,66 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2627,21 +2617,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E83" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E83" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
   <autoFilter ref="A1:E83"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Module" dataDxfId="38"/>
-    <tableColumn id="2" name="Task" dataDxfId="37"/>
+    <tableColumn id="1" name="Module" dataDxfId="24"/>
+    <tableColumn id="2" name="Task" dataDxfId="23"/>
     <tableColumn id="6" name="Priority"/>
-    <tableColumn id="3" name="Owner" dataDxfId="36"/>
-    <tableColumn id="5" name="EE" dataDxfId="35"/>
+    <tableColumn id="3" name="Owner" dataDxfId="22"/>
+    <tableColumn id="5" name="EE" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:E100" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:E100" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A1:E100"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Module"/>
@@ -2655,7 +2645,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:E100" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:E100" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:E100"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Module"/>
@@ -2669,7 +2659,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table158" displayName="Table158" ref="A1:E100" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table158" displayName="Table158" ref="A1:E100" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:E100"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Module"/>
@@ -2985,7 +2975,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3009,48 +2999,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="148" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="144" t="s">
+      <c r="B1" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="144" t="s">
+      <c r="C1" s="148" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="144" t="s">
+      <c r="D1" s="148" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="150" t="s">
+      <c r="E1" s="153" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="142"/>
-      <c r="G1" s="141" t="s">
+      <c r="F1" s="152"/>
+      <c r="G1" s="151" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="142"/>
-      <c r="I1" s="141" t="s">
+      <c r="H1" s="152"/>
+      <c r="I1" s="151" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="142"/>
-      <c r="K1" s="141" t="s">
+      <c r="J1" s="152"/>
+      <c r="K1" s="151" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="142"/>
-      <c r="M1" s="141" t="s">
+      <c r="L1" s="152"/>
+      <c r="M1" s="151" t="s">
         <v>148</v>
       </c>
-      <c r="N1" s="142"/>
-      <c r="O1" s="141" t="s">
+      <c r="N1" s="152"/>
+      <c r="O1" s="151" t="s">
         <v>149</v>
       </c>
-      <c r="P1" s="142"/>
+      <c r="P1" s="152"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="143"/>
+      <c r="A2" s="149"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="150"/>
       <c r="E2" s="90" t="s">
         <v>111</v>
       </c>
@@ -3089,7 +3079,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="141" t="s">
         <v>81</v>
       </c>
       <c r="B3" s="83" t="s">
@@ -3135,7 +3125,7 @@
       <c r="P3" s="87"/>
     </row>
     <row r="4" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="146" t="s">
+      <c r="A4" s="141" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="83" t="s">
@@ -3181,7 +3171,7 @@
       <c r="P4" s="87"/>
     </row>
     <row r="5" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="146" t="s">
+      <c r="A5" s="141" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="83" t="s">
@@ -3226,7 +3216,7 @@
       <c r="P5" s="87"/>
     </row>
     <row r="6" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="146" t="s">
+      <c r="A6" s="141" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="83" t="s">
@@ -3272,7 +3262,7 @@
       <c r="P6" s="87"/>
     </row>
     <row r="7" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="141" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="83" t="s">
@@ -3318,7 +3308,7 @@
       <c r="P7" s="87"/>
     </row>
     <row r="8" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="146" t="s">
+      <c r="A8" s="141" t="s">
         <v>88</v>
       </c>
       <c r="B8" s="83" t="s">
@@ -3364,13 +3354,15 @@
       <c r="P8" s="87"/>
     </row>
     <row r="9" spans="1:16" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147" t="s">
+      <c r="A9" s="142" t="s">
         <v>90</v>
       </c>
       <c r="B9" s="138" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="139"/>
+      <c r="C9" s="139">
+        <v>61467109</v>
+      </c>
       <c r="D9" s="140" t="s">
         <v>91</v>
       </c>
@@ -3408,51 +3400,51 @@
       <c r="P9" s="87"/>
     </row>
     <row r="10" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="148" t="s">
+      <c r="A10" s="143" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="149"/>
-      <c r="C10" s="149"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="152">
+      <c r="B10" s="144"/>
+      <c r="C10" s="144"/>
+      <c r="D10" s="145"/>
+      <c r="E10" s="146">
         <f>SUM(E3:E9)*6</f>
         <v>0</v>
       </c>
-      <c r="F10" s="153">
+      <c r="F10" s="147">
         <f>RIGHT(E$1, (LEN(E$1)-FIND("_", E$1)))+RIGHT(E$1, (LEN(E$1)-FIND("_", E$1)))*0.3+RIGHT(E$1, (LEN(E$1)-FIND("_", E$1)))*0.65-E$10</f>
         <v>234</v>
       </c>
-      <c r="G10" s="152">
+      <c r="G10" s="146">
         <f>SUM(G3:G9)*6</f>
         <v>72</v>
       </c>
-      <c r="H10" s="153">
+      <c r="H10" s="147">
         <f>RIGHT(G$1, (LEN(G$1)-FIND("_", G$1)))*1+RIGHT(G$1, (LEN(G$1)-FIND("_", G$1)))*4*0.8+RIGHT(G$1, (LEN(G$1)-FIND("_", G$1)))*0.65-G$10</f>
         <v>655.5</v>
       </c>
-      <c r="I10" s="152">
+      <c r="I10" s="146">
         <f>SUM(I3:I9)*6</f>
         <v>0</v>
       </c>
-      <c r="J10" s="153">
+      <c r="J10" s="147">
         <f>RIGHT(I$1, (LEN(I$1)-FIND("_", I$1)))*6+RIGHT(I$1, (LEN(I$1)-FIND("_", I$1)))*0.65-I$10</f>
         <v>798</v>
       </c>
-      <c r="K10" s="152">
+      <c r="K10" s="146">
         <f>SUM(K3:K9)*6</f>
         <v>0</v>
       </c>
-      <c r="L10" s="153">
+      <c r="L10" s="147">
         <f>RIGHT(K$1, (LEN(K$1)-FIND("_", K$1)))*6+RIGHT(K$1, (LEN(K$1)-FIND("_", K$1)))*0.65-K$10</f>
         <v>798</v>
       </c>
-      <c r="M10" s="152"/>
-      <c r="N10" s="153">
+      <c r="M10" s="146"/>
+      <c r="N10" s="147">
         <f>RIGHT(M$1, (LEN(M$1)-FIND("_", M$1)))*6+RIGHT(M$1, (LEN(M$1)-FIND("_", M$1)))*0.65-M$10</f>
         <v>798</v>
       </c>
-      <c r="O10" s="152"/>
-      <c r="P10" s="153">
+      <c r="O10" s="146"/>
+      <c r="P10" s="147">
         <f>RIGHT(O$1, (LEN(O$1)-FIND("_", O$1)))*6+RIGHT(O$1, (LEN(O$1)-FIND("_", O$1)))*0.65-O$10</f>
         <v>798</v>
       </c>
@@ -3462,67 +3454,67 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F3:F9 F11:F100">
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="39" priority="27">
       <formula>IF(AND(F3&gt;=(108-(E3*6)),F3&lt;(120-(E3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="30">
+    <cfRule type="expression" dxfId="38" priority="30">
       <formula>IF(F3&gt;=(120 - E3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J9">
-    <cfRule type="expression" dxfId="23" priority="9">
+    <cfRule type="expression" dxfId="37" priority="9">
       <formula>IF(AND(J3&gt;=(108-(I3*6)),J3&lt;(120-(I3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="10">
+    <cfRule type="expression" dxfId="36" priority="10">
       <formula>IF(J3&gt;=(120 - I3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L9">
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="35" priority="7">
       <formula>IF(AND(L3&gt;=(108-(K3*6)),L3&lt;(120-(K3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="34" priority="8">
       <formula>IF(L3&gt;=(120 - K3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="19" priority="6">
+    <cfRule type="expression" dxfId="33" priority="6">
       <formula>IF(F3&gt;=(120*0.65-(E3*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H9">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>IF(AND(H3&gt;=(108-(G3*6)),H3&lt;(120-(G3*6))),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="31" priority="5">
       <formula>IF(H3&gt;=(120 - G3*6), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="30" priority="3">
       <formula>IF(H3&gt;=(120*0.65-(G3*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>IF(H4&gt;=(120*0.65-(G4*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>IF(H3&gt;=(120*0.65-(G3*6)),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5137,22 +5129,22 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I56:I57">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H58">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F58">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>IF(#REF!=1, 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E100">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>IF($C2=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5756,22 +5748,22 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I56:I57">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H58">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F58">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>IF(#REF!=1, 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E100">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>IF($C2=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6376,22 +6368,22 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I56:I57">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H58">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>IF(#REF!=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F58">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>IF(#REF!=1, 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E100">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>IF($C2=1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>